<commit_message>
Fix compositions with fractions
</commit_message>
<xml_diff>
--- a/24-10_Contributions.xlsx
+++ b/24-10_Contributions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardonpa/Library/CloudStorage/GoogleDrive-ricardo.npa@gmail.com/Shared drives/Development/Codes/ULTERA-contribute-rdamaral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DB8F68-D36E-5C4E-91E2-642920B25437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F1244-E5E1-6045-AB19-52110562ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="500" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,12 +380,6 @@
     <t>V Nb Ta Mo</t>
   </si>
   <si>
-    <t>V1/3.8 Nb1/3.8 Ta1/3.8 Mo0.8/3.8</t>
-  </si>
-  <si>
-    <t>V1/4.2 Nb1/4.2 Ta1/4.2 Mo1.2/4.2</t>
-  </si>
-  <si>
     <t>F6</t>
   </si>
   <si>
@@ -401,15 +395,6 @@
     <t>Fe Co Cr Ni</t>
   </si>
   <si>
-    <t>Fe1/4.1 Co1/4.1 Cr1/4.1 Ni1/4.1 Mo0.1/4.1</t>
-  </si>
-  <si>
-    <t>Fe1/4.3 Co1/4.3 Cr1/4.3 Ni1/4.3 Mo0.3/4.3</t>
-  </si>
-  <si>
-    <t>Fe1/4.5 Co1/4.5 Cr1/4.5 Ni1/4.5 Mo0.5/4.5</t>
-  </si>
-  <si>
     <t>total tensile ductility</t>
   </si>
   <si>
@@ -437,9 +422,6 @@
     <t>T4</t>
   </si>
   <si>
-    <t>Al1/5 Mo0.5/5 Nb1/5 Ta0.5/5 Ti1/5 Zr1/5</t>
-  </si>
-  <si>
     <t>Al Nb Ta Ti Zr</t>
   </si>
   <si>
@@ -450,6 +432,24 @@
   </si>
   <si>
     <t>10.1016/j.jallcom.2024.177079</t>
+  </si>
+  <si>
+    <t>V0.263 Nb0.263 Ta0.263 Mo0.211</t>
+  </si>
+  <si>
+    <t>V0.238 Nb0.238 Ta0.238 Mo0.286</t>
+  </si>
+  <si>
+    <t>Fe0.244 Co0.244 Cr0.244 Ni0.244 Mo0.024</t>
+  </si>
+  <si>
+    <t>Fe0.233 Co0.233 Cr0.233 Ni0.233 Mo0.07</t>
+  </si>
+  <si>
+    <t>Fe0.222 Co0.222 Cr0.222 Ni0.222 Mo0.111</t>
+  </si>
+  <si>
+    <t>Al0.2 Mo0.1 Nb0.2 Ta0.1 Ti0.2 Zr0.2</t>
   </si>
 </sst>
 </file>
@@ -1123,6 +1123,33 @@
     <xf numFmtId="11" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1174,34 +1201,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1488,7 +1488,7 @@
   <dimension ref="A1:T206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="P10" sqref="P10:Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,19 +1523,19 @@
       <c r="B2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1545,17 +1545,17 @@
       <c r="B3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1573,43 +1573,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="57" t="s">
+      <c r="L5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="40" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1620,19 +1620,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="60"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1677,7 +1677,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="61"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -1690,35 +1690,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="54" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="62" t="s">
+      <c r="P8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="64"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1818,10 +1818,10 @@
         <v>44</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -1860,10 +1860,10 @@
         <v>63</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
@@ -1871,7 +1871,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>68</v>
@@ -1904,10 +1904,10 @@
         <v>44</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
@@ -1915,7 +1915,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>68</v>
@@ -1946,10 +1946,10 @@
         <v>63</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
@@ -1957,7 +1957,7 @@
         <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>68</v>
@@ -1990,10 +1990,10 @@
         <v>44</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N14" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
@@ -2001,7 +2001,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>68</v>
@@ -2032,10 +2032,10 @@
         <v>63</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
@@ -2062,7 +2062,7 @@
         <v>64</v>
       </c>
       <c r="I16" s="34">
-        <f>1500+273</f>
+        <f t="shared" ref="I16:I21" si="0">1500+273</f>
         <v>1773</v>
       </c>
       <c r="J16" s="31">
@@ -2077,7 +2077,7 @@
         <v>79</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -2101,10 +2101,10 @@
         <v>19</v>
       </c>
       <c r="H17" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I17" s="34">
-        <f>1500+273</f>
+        <f t="shared" si="0"/>
         <v>1773</v>
       </c>
       <c r="J17" s="31">
@@ -2119,7 +2119,7 @@
         <v>79</v>
       </c>
       <c r="N17" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2127,7 +2127,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>68</v>
@@ -2146,7 +2146,7 @@
         <v>64</v>
       </c>
       <c r="I18" s="34">
-        <f>1500+273</f>
+        <f t="shared" si="0"/>
         <v>1773</v>
       </c>
       <c r="J18" s="31">
@@ -2161,7 +2161,7 @@
         <v>79</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2169,7 +2169,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>68</v>
@@ -2185,10 +2185,10 @@
         <v>19</v>
       </c>
       <c r="H19" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I19" s="34">
-        <f>1500+273</f>
+        <f t="shared" si="0"/>
         <v>1773</v>
       </c>
       <c r="J19" s="31">
@@ -2203,7 +2203,7 @@
         <v>79</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2211,7 +2211,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>68</v>
@@ -2230,7 +2230,7 @@
         <v>64</v>
       </c>
       <c r="I20" s="34">
-        <f>1500+273</f>
+        <f t="shared" si="0"/>
         <v>1773</v>
       </c>
       <c r="J20" s="31">
@@ -2245,7 +2245,7 @@
         <v>79</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -2253,7 +2253,7 @@
         <v>82</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>68</v>
@@ -2269,10 +2269,10 @@
         <v>19</v>
       </c>
       <c r="H21" s="32" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I21" s="34">
-        <f>1500+273</f>
+        <f t="shared" si="0"/>
         <v>1773</v>
       </c>
       <c r="J21" s="31">
@@ -2287,15 +2287,15 @@
         <v>79</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C22" s="32" t="s">
         <v>71</v>
@@ -2313,7 +2313,7 @@
         <v>19</v>
       </c>
       <c r="H22" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I22" s="34">
         <f>25+273</f>
@@ -2331,15 +2331,15 @@
         <v>65</v>
       </c>
       <c r="N22" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C23" s="32" t="s">
         <v>71</v>
@@ -2357,10 +2357,10 @@
         <v>19</v>
       </c>
       <c r="H23" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I23" s="34">
-        <f t="shared" ref="I23:I25" si="0">25+273</f>
+        <f t="shared" ref="I23:I25" si="1">25+273</f>
         <v>298</v>
       </c>
       <c r="J23" s="31">
@@ -2375,15 +2375,15 @@
         <v>65</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>71</v>
@@ -2401,10 +2401,10 @@
         <v>19</v>
       </c>
       <c r="H24" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I24" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>298</v>
       </c>
       <c r="J24" s="31">
@@ -2418,15 +2418,15 @@
         <v>65</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C25" s="32" t="s">
         <v>71</v>
@@ -2438,16 +2438,16 @@
         <v>77</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H25" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I25" s="34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>298</v>
       </c>
       <c r="J25" s="31">
@@ -2461,15 +2461,15 @@
         <v>65</v>
       </c>
       <c r="N25" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C26" s="32" t="s">
         <v>71</v>
@@ -2487,7 +2487,7 @@
         <v>19</v>
       </c>
       <c r="H26" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I26" s="34">
         <f>600+273</f>
@@ -2505,15 +2505,15 @@
         <v>65</v>
       </c>
       <c r="N26" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C27" s="32" t="s">
         <v>71</v>
@@ -2531,10 +2531,10 @@
         <v>19</v>
       </c>
       <c r="H27" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I27" s="34">
-        <f t="shared" ref="I27:I29" si="1">600+273</f>
+        <f t="shared" ref="I27:I29" si="2">600+273</f>
         <v>873</v>
       </c>
       <c r="J27" s="31">
@@ -2549,15 +2549,15 @@
         <v>65</v>
       </c>
       <c r="N27" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C28" s="32" t="s">
         <v>71</v>
@@ -2575,10 +2575,10 @@
         <v>19</v>
       </c>
       <c r="H28" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I28" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>873</v>
       </c>
       <c r="J28" s="31">
@@ -2592,15 +2592,15 @@
         <v>65</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C29" s="32" t="s">
         <v>71</v>
@@ -2612,16 +2612,16 @@
         <v>77</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I29" s="34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>873</v>
       </c>
       <c r="J29" s="31">
@@ -2635,15 +2635,15 @@
         <v>65</v>
       </c>
       <c r="N29" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>72</v>
@@ -2661,10 +2661,10 @@
         <v>19</v>
       </c>
       <c r="H30" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I30" s="34">
-        <f t="shared" ref="I30:I49" si="2">25+273</f>
+        <f t="shared" ref="I30:I49" si="3">25+273</f>
         <v>298</v>
       </c>
       <c r="J30" s="31">
@@ -2679,15 +2679,15 @@
         <v>65</v>
       </c>
       <c r="N30" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>72</v>
@@ -2705,10 +2705,10 @@
         <v>19</v>
       </c>
       <c r="H31" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I31" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J31" s="31">
@@ -2723,15 +2723,15 @@
         <v>65</v>
       </c>
       <c r="N31" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>72</v>
@@ -2749,10 +2749,10 @@
         <v>19</v>
       </c>
       <c r="H32" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I32" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J32" s="31">
@@ -2766,15 +2766,15 @@
         <v>65</v>
       </c>
       <c r="N32" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>72</v>
@@ -2786,16 +2786,16 @@
         <v>77</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G33" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H33" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I33" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J33" s="31">
@@ -2809,15 +2809,15 @@
         <v>65</v>
       </c>
       <c r="N33" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C34" s="33" t="s">
         <v>72</v>
@@ -2835,10 +2835,10 @@
         <v>19</v>
       </c>
       <c r="H34" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I34" s="34">
-        <f t="shared" ref="I34:I53" si="3">600+273</f>
+        <f t="shared" ref="I34:I53" si="4">600+273</f>
         <v>873</v>
       </c>
       <c r="J34" s="31">
@@ -2853,15 +2853,15 @@
         <v>65</v>
       </c>
       <c r="N34" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>72</v>
@@ -2879,10 +2879,10 @@
         <v>19</v>
       </c>
       <c r="H35" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I35" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J35" s="31">
@@ -2897,15 +2897,15 @@
         <v>65</v>
       </c>
       <c r="N35" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>72</v>
@@ -2923,10 +2923,10 @@
         <v>19</v>
       </c>
       <c r="H36" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I36" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J36" s="31">
@@ -2940,15 +2940,15 @@
         <v>65</v>
       </c>
       <c r="N36" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>72</v>
@@ -2960,16 +2960,16 @@
         <v>77</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G37" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H37" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I37" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J37" s="31">
@@ -2983,15 +2983,15 @@
         <v>65</v>
       </c>
       <c r="N37" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>72</v>
@@ -3009,10 +3009,10 @@
         <v>19</v>
       </c>
       <c r="H38" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I38" s="34">
-        <f t="shared" ref="I38" si="4">25+273</f>
+        <f t="shared" ref="I38" si="5">25+273</f>
         <v>298</v>
       </c>
       <c r="J38" s="31">
@@ -3027,15 +3027,15 @@
         <v>65</v>
       </c>
       <c r="N38" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>72</v>
@@ -3053,10 +3053,10 @@
         <v>19</v>
       </c>
       <c r="H39" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I39" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J39" s="31">
@@ -3071,15 +3071,15 @@
         <v>65</v>
       </c>
       <c r="N39" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>72</v>
@@ -3097,10 +3097,10 @@
         <v>19</v>
       </c>
       <c r="H40" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I40" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J40" s="31">
@@ -3114,15 +3114,15 @@
         <v>65</v>
       </c>
       <c r="N40" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>72</v>
@@ -3134,16 +3134,16 @@
         <v>77</v>
       </c>
       <c r="F41" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G41" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H41" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I41" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J41" s="31">
@@ -3157,15 +3157,15 @@
         <v>65</v>
       </c>
       <c r="N41" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>72</v>
@@ -3183,10 +3183,10 @@
         <v>19</v>
       </c>
       <c r="H42" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I42" s="34">
-        <f t="shared" ref="I42" si="5">600+273</f>
+        <f t="shared" ref="I42" si="6">600+273</f>
         <v>873</v>
       </c>
       <c r="J42" s="31">
@@ -3201,15 +3201,15 @@
         <v>65</v>
       </c>
       <c r="N42" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>72</v>
@@ -3227,10 +3227,10 @@
         <v>19</v>
       </c>
       <c r="H43" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I43" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J43" s="31">
@@ -3245,15 +3245,15 @@
         <v>65</v>
       </c>
       <c r="N43" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>72</v>
@@ -3271,10 +3271,10 @@
         <v>19</v>
       </c>
       <c r="H44" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I44" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J44" s="31">
@@ -3288,15 +3288,15 @@
         <v>65</v>
       </c>
       <c r="N44" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>72</v>
@@ -3308,16 +3308,16 @@
         <v>77</v>
       </c>
       <c r="F45" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G45" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H45" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I45" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J45" s="31">
@@ -3331,15 +3331,15 @@
         <v>65</v>
       </c>
       <c r="N45" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>72</v>
@@ -3357,10 +3357,10 @@
         <v>19</v>
       </c>
       <c r="H46" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I46" s="34">
-        <f t="shared" ref="I46" si="6">25+273</f>
+        <f t="shared" ref="I46" si="7">25+273</f>
         <v>298</v>
       </c>
       <c r="J46" s="31">
@@ -3375,15 +3375,15 @@
         <v>65</v>
       </c>
       <c r="N46" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>72</v>
@@ -3401,10 +3401,10 @@
         <v>19</v>
       </c>
       <c r="H47" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I47" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J47" s="31">
@@ -3419,15 +3419,15 @@
         <v>65</v>
       </c>
       <c r="N47" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>72</v>
@@ -3445,10 +3445,10 @@
         <v>19</v>
       </c>
       <c r="H48" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I48" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J48" s="31">
@@ -3462,15 +3462,15 @@
         <v>65</v>
       </c>
       <c r="N48" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>72</v>
@@ -3482,16 +3482,16 @@
         <v>77</v>
       </c>
       <c r="F49" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G49" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H49" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I49" s="34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>298</v>
       </c>
       <c r="J49" s="31">
@@ -3505,15 +3505,15 @@
         <v>65</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>72</v>
@@ -3531,10 +3531,10 @@
         <v>19</v>
       </c>
       <c r="H50" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I50" s="34">
-        <f t="shared" ref="I50" si="7">600+273</f>
+        <f t="shared" ref="I50" si="8">600+273</f>
         <v>873</v>
       </c>
       <c r="J50" s="31">
@@ -3549,15 +3549,15 @@
         <v>65</v>
       </c>
       <c r="N50" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>72</v>
@@ -3575,10 +3575,10 @@
         <v>19</v>
       </c>
       <c r="H51" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I51" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J51" s="31">
@@ -3593,15 +3593,15 @@
         <v>65</v>
       </c>
       <c r="N51" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>72</v>
@@ -3619,10 +3619,10 @@
         <v>19</v>
       </c>
       <c r="H52" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I52" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J52" s="31">
@@ -3636,15 +3636,15 @@
         <v>65</v>
       </c>
       <c r="N52" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="35" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>72</v>
@@ -3656,16 +3656,16 @@
         <v>77</v>
       </c>
       <c r="F53" s="32" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G53" s="32" t="s">
         <v>19</v>
       </c>
       <c r="H53" s="32" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I53" s="34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>873</v>
       </c>
       <c r="J53" s="31">
@@ -3679,7 +3679,7 @@
         <v>65</v>
       </c>
       <c r="N53" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -3687,7 +3687,7 @@
         <v>3</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>78</v>
@@ -3724,7 +3724,7 @@
         <v>79</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -3732,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>78</v>
@@ -3742,7 +3742,7 @@
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>19</v>
@@ -3767,7 +3767,7 @@
         <v>79</v>
       </c>
       <c r="N55" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -3775,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>78</v>
@@ -3812,7 +3812,7 @@
         <v>79</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3820,7 +3820,7 @@
         <v>3</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C57" s="33" t="s">
         <v>78</v>
@@ -3830,7 +3830,7 @@
       </c>
       <c r="E57" s="19"/>
       <c r="F57" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>19</v>
@@ -3843,7 +3843,7 @@
         <v>1473</v>
       </c>
       <c r="J57" s="31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K57" s="31"/>
       <c r="L57" s="19" t="s">
@@ -3853,7 +3853,7 @@
         <v>79</v>
       </c>
       <c r="N57" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -3861,7 +3861,7 @@
         <v>3</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>78</v>
@@ -3898,7 +3898,7 @@
         <v>79</v>
       </c>
       <c r="N58" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -3906,7 +3906,7 @@
         <v>3</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C59" s="33" t="s">
         <v>78</v>
@@ -3916,7 +3916,7 @@
       </c>
       <c r="E59" s="19"/>
       <c r="F59" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G59" s="32" t="s">
         <v>19</v>
@@ -3929,7 +3929,7 @@
         <v>1873</v>
       </c>
       <c r="J59" s="31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K59" s="31"/>
       <c r="L59" s="19" t="s">
@@ -3939,7 +3939,7 @@
         <v>79</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -3947,7 +3947,7 @@
         <v>3</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C60" s="33" t="s">
         <v>78</v>
@@ -3984,7 +3984,7 @@
         <v>79</v>
       </c>
       <c r="N60" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -3992,7 +3992,7 @@
         <v>3</v>
       </c>
       <c r="B61" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C61" s="33" t="s">
         <v>78</v>
@@ -4002,7 +4002,7 @@
       </c>
       <c r="E61" s="19"/>
       <c r="F61" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G61" s="32" t="s">
         <v>19</v>
@@ -4015,7 +4015,7 @@
         <v>2073</v>
       </c>
       <c r="J61" s="31" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="K61" s="31"/>
       <c r="L61" s="19" t="s">
@@ -4025,7 +4025,7 @@
         <v>79</v>
       </c>
       <c r="N61" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -4033,7 +4033,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C62" s="33" t="s">
         <v>78</v>
@@ -4062,10 +4062,10 @@
         <v>44</v>
       </c>
       <c r="M62" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N62" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -4073,7 +4073,7 @@
         <v>3</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C63" s="33" t="s">
         <v>78</v>
@@ -4101,10 +4101,10 @@
         <v>81</v>
       </c>
       <c r="M63" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="N63" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -4112,7 +4112,7 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C64" s="33" t="s">
         <v>68</v>
@@ -4148,7 +4148,7 @@
         <v>79</v>
       </c>
       <c r="N64" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -4156,7 +4156,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C65" s="33" t="s">
         <v>68</v>
@@ -4165,7 +4165,7 @@
         <v>61</v>
       </c>
       <c r="F65" s="32" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G65" s="32" t="s">
         <v>19</v>
@@ -4190,7 +4190,7 @@
         <v>79</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -4198,10 +4198,10 @@
         <v>4</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D66" s="32" t="s">
         <v>75</v>
@@ -4227,10 +4227,10 @@
         <v>44</v>
       </c>
       <c r="M66" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4238,10 +4238,10 @@
         <v>4</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D67" s="32" t="s">
         <v>75</v>
@@ -4271,10 +4271,10 @@
         <v>44</v>
       </c>
       <c r="M67" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="N67" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4282,10 +4282,10 @@
         <v>4</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C68" s="33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D68" s="32" t="s">
         <v>75</v>
@@ -4312,10 +4312,10 @@
         <v>44</v>
       </c>
       <c r="M68" s="19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N68" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4323,10 +4323,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D69" s="32" t="s">
         <v>75</v>
@@ -4356,10 +4356,10 @@
         <v>44</v>
       </c>
       <c r="M69" s="19" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="N69" s="19" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -5990,11 +5990,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -6009,6 +6004,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix to `24-10` Contributions
</commit_message>
<xml_diff>
--- a/24-10_Contributions.xlsx
+++ b/24-10_Contributions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardonpa/Library/CloudStorage/GoogleDrive-ricardo.npa@gmail.com/Shared drives/Development/Codes/ULTERA-contribute-rdamaral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83F1244-E5E1-6045-AB19-52110562ECFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119AE11-2942-EC4B-8509-6BC50BE494A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1123,6 +1123,63 @@
     <xf numFmtId="11" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1141,67 +1198,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1487,8 +1487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10:Q69"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,19 +1523,19 @@
       <c r="B2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1545,17 +1545,17 @@
       <c r="B3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1573,43 +1573,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="M5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="59" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1620,19 +1620,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="41"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="60"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1677,7 +1677,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="61"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -1690,35 +1690,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="43" t="s">
+      <c r="P8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="45"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="64"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1807,12 +1807,12 @@
         <v>298</v>
       </c>
       <c r="J10" s="31">
-        <f>1326*10000000</f>
-        <v>13260000000</v>
+        <f>1326*10^6</f>
+        <v>1326000000</v>
       </c>
       <c r="K10" s="31">
-        <f>32*10000000</f>
-        <v>320000000</v>
+        <f>32*10^6</f>
+        <v>32000000</v>
       </c>
       <c r="L10" s="19" t="s">
         <v>44</v>
@@ -1893,12 +1893,12 @@
         <v>298</v>
       </c>
       <c r="J12" s="31">
-        <f>1214*10000000</f>
-        <v>12140000000</v>
+        <f>1214*10^6</f>
+        <v>1214000000</v>
       </c>
       <c r="K12" s="31">
-        <f>26*10000000</f>
-        <v>260000000</v>
+        <f>26*10^6</f>
+        <v>26000000</v>
       </c>
       <c r="L12" s="19" t="s">
         <v>44</v>
@@ -1979,12 +1979,12 @@
         <v>298</v>
       </c>
       <c r="J14" s="31">
-        <f>1465*10000000</f>
-        <v>14650000000</v>
+        <f>1465*10^6</f>
+        <v>1465000000</v>
       </c>
       <c r="K14" s="31">
-        <f>39*10000000</f>
-        <v>390000000</v>
+        <f>39*10^6</f>
+        <v>39000000</v>
       </c>
       <c r="L14" s="19" t="s">
         <v>44</v>
@@ -2066,8 +2066,8 @@
         <v>1773</v>
       </c>
       <c r="J16" s="31">
-        <f>381.74*10000000</f>
-        <v>3817400000</v>
+        <f>381.74*10^6</f>
+        <v>381740000</v>
       </c>
       <c r="K16" s="31"/>
       <c r="L16" s="19" t="s">
@@ -2108,8 +2108,8 @@
         <v>1773</v>
       </c>
       <c r="J17" s="31">
-        <f>534.92*10000000</f>
-        <v>5349200000</v>
+        <f>534.92*10^6</f>
+        <v>534919999.99999994</v>
       </c>
       <c r="K17" s="31"/>
       <c r="L17" s="19" t="s">
@@ -2150,8 +2150,8 @@
         <v>1773</v>
       </c>
       <c r="J18" s="31">
-        <f>335.47*10000000</f>
-        <v>3354700000.0000005</v>
+        <f>335.47*10^6</f>
+        <v>335470000</v>
       </c>
       <c r="K18" s="31"/>
       <c r="L18" s="19" t="s">
@@ -2192,8 +2192,8 @@
         <v>1773</v>
       </c>
       <c r="J19" s="31">
-        <f>433.79*10000000</f>
-        <v>4337900000</v>
+        <f>433.79*10^6</f>
+        <v>433790000</v>
       </c>
       <c r="K19" s="31"/>
       <c r="L19" s="19" t="s">
@@ -2234,8 +2234,8 @@
         <v>1773</v>
       </c>
       <c r="J20" s="31">
-        <f>412.57*10000000</f>
-        <v>4125700000</v>
+        <f>412.57*10^6</f>
+        <v>412570000</v>
       </c>
       <c r="K20" s="31"/>
       <c r="L20" s="19" t="s">
@@ -2276,8 +2276,8 @@
         <v>1773</v>
       </c>
       <c r="J21" s="31">
-        <f>577.87*10000000</f>
-        <v>5778700000</v>
+        <f>577.87*10^6</f>
+        <v>577870000</v>
       </c>
       <c r="K21" s="31"/>
       <c r="L21" s="19" t="s">
@@ -2320,8 +2320,8 @@
         <v>298</v>
       </c>
       <c r="J22" s="31">
-        <f>533*10000000</f>
-        <v>5330000000</v>
+        <f>533*10^6</f>
+        <v>533000000</v>
       </c>
       <c r="K22" s="31"/>
       <c r="L22" s="19" t="s">
@@ -2364,8 +2364,8 @@
         <v>298</v>
       </c>
       <c r="J23" s="31">
-        <f>719*10000000</f>
-        <v>7190000000</v>
+        <f>719*10^6</f>
+        <v>719000000</v>
       </c>
       <c r="K23" s="31"/>
       <c r="L23" s="19" t="s">
@@ -2494,8 +2494,8 @@
         <v>873</v>
       </c>
       <c r="J26" s="31">
-        <f>398*10000000</f>
-        <v>3980000000</v>
+        <f>398*10^6</f>
+        <v>398000000</v>
       </c>
       <c r="K26" s="31"/>
       <c r="L26" s="19" t="s">
@@ -2538,8 +2538,8 @@
         <v>873</v>
       </c>
       <c r="J27" s="31">
-        <f>420*10000000</f>
-        <v>4200000000</v>
+        <f>420*10^6</f>
+        <v>420000000</v>
       </c>
       <c r="K27" s="31"/>
       <c r="L27" s="19" t="s">
@@ -2668,8 +2668,8 @@
         <v>298</v>
       </c>
       <c r="J30" s="31">
-        <f>609*10000000</f>
-        <v>6090000000</v>
+        <f>609*10^6</f>
+        <v>609000000</v>
       </c>
       <c r="K30" s="31"/>
       <c r="L30" s="19" t="s">
@@ -2712,8 +2712,8 @@
         <v>298</v>
       </c>
       <c r="J31" s="31">
-        <f>776*10000000</f>
-        <v>7760000000</v>
+        <f>776*10^6</f>
+        <v>776000000</v>
       </c>
       <c r="K31" s="31"/>
       <c r="L31" s="19" t="s">
@@ -2842,8 +2842,8 @@
         <v>873</v>
       </c>
       <c r="J34" s="31">
-        <f>407*10000000</f>
-        <v>4070000000</v>
+        <f>407*10^6</f>
+        <v>407000000</v>
       </c>
       <c r="K34" s="31"/>
       <c r="L34" s="19" t="s">
@@ -2886,8 +2886,8 @@
         <v>873</v>
       </c>
       <c r="J35" s="31">
-        <f>473*10000000</f>
-        <v>4730000000</v>
+        <f>473*10^6</f>
+        <v>473000000</v>
       </c>
       <c r="K35" s="31"/>
       <c r="L35" s="19" t="s">
@@ -3016,8 +3016,8 @@
         <v>298</v>
       </c>
       <c r="J38" s="31">
-        <f>698*10000000</f>
-        <v>6980000000</v>
+        <f>698*10^6</f>
+        <v>698000000</v>
       </c>
       <c r="K38" s="31"/>
       <c r="L38" s="19" t="s">
@@ -3060,8 +3060,8 @@
         <v>298</v>
       </c>
       <c r="J39" s="31">
-        <f>953*10000000</f>
-        <v>9530000000</v>
+        <f>953*10^6</f>
+        <v>953000000</v>
       </c>
       <c r="K39" s="31"/>
       <c r="L39" s="19" t="s">
@@ -3190,8 +3190,8 @@
         <v>873</v>
       </c>
       <c r="J42" s="31">
-        <f>477*10000000</f>
-        <v>4770000000</v>
+        <f>477*10^6</f>
+        <v>477000000</v>
       </c>
       <c r="K42" s="31"/>
       <c r="L42" s="19" t="s">
@@ -3234,8 +3234,8 @@
         <v>873</v>
       </c>
       <c r="J43" s="31">
-        <f>661*10000000</f>
-        <v>6610000000</v>
+        <f>661*10^6</f>
+        <v>661000000</v>
       </c>
       <c r="K43" s="31"/>
       <c r="L43" s="19" t="s">
@@ -3364,8 +3364,8 @@
         <v>298</v>
       </c>
       <c r="J46" s="31">
-        <f>930*10000000</f>
-        <v>9300000000</v>
+        <f>930*10^6</f>
+        <v>930000000</v>
       </c>
       <c r="K46" s="31"/>
       <c r="L46" s="19" t="s">
@@ -3408,8 +3408,8 @@
         <v>298</v>
       </c>
       <c r="J47" s="31">
-        <f>1091*10000000</f>
-        <v>10910000000</v>
+        <f>1091*10^6</f>
+        <v>1091000000</v>
       </c>
       <c r="K47" s="31"/>
       <c r="L47" s="19" t="s">
@@ -3538,8 +3538,8 @@
         <v>873</v>
       </c>
       <c r="J50" s="31">
-        <f>578*10000000</f>
-        <v>5780000000</v>
+        <f>578*10^6</f>
+        <v>578000000</v>
       </c>
       <c r="K50" s="31"/>
       <c r="L50" s="19" t="s">
@@ -3582,8 +3582,8 @@
         <v>873</v>
       </c>
       <c r="J51" s="31">
-        <f>799*10000000</f>
-        <v>7990000000</v>
+        <f>799*10^6</f>
+        <v>799000000</v>
       </c>
       <c r="K51" s="31"/>
       <c r="L51" s="19" t="s">
@@ -3710,8 +3710,8 @@
         <v>298</v>
       </c>
       <c r="J54" s="31">
-        <f>1730*10000000</f>
-        <v>17300000000</v>
+        <f>1730*10^6</f>
+        <v>1730000000</v>
       </c>
       <c r="K54" s="31">
         <f>22*10000000</f>
@@ -3798,8 +3798,8 @@
         <v>1473</v>
       </c>
       <c r="J56" s="31">
-        <f>1088*10000000</f>
-        <v>10880000000</v>
+        <f>1088*10^6</f>
+        <v>1088000000</v>
       </c>
       <c r="K56" s="31">
         <f>26*10000000</f>
@@ -3884,8 +3884,8 @@
         <v>1873</v>
       </c>
       <c r="J58" s="31">
-        <f>390*10000000</f>
-        <v>3900000000</v>
+        <f>390*10^6</f>
+        <v>390000000</v>
       </c>
       <c r="K58" s="31">
         <f>18*10000000</f>
@@ -3970,8 +3970,8 @@
         <v>2073</v>
       </c>
       <c r="J60" s="31">
-        <f>312*10000000</f>
-        <v>3120000000</v>
+        <f>312*10^6</f>
+        <v>312000000</v>
       </c>
       <c r="K60" s="31">
         <f>16*10000000</f>
@@ -4054,8 +4054,8 @@
         <v>298</v>
       </c>
       <c r="J62" s="31">
-        <f>3.58*10000000000</f>
-        <v>35800000000</v>
+        <f>3.58*10^9</f>
+        <v>3580000000</v>
       </c>
       <c r="K62" s="31"/>
       <c r="L62" s="19" t="s">
@@ -4134,8 +4134,8 @@
         <v>298</v>
       </c>
       <c r="J64" s="31">
-        <f>1042*10000000</f>
-        <v>10420000000</v>
+        <f>1042*10^6</f>
+        <v>1042000000</v>
       </c>
       <c r="K64" s="31">
         <f>41*10000000</f>
@@ -4219,8 +4219,8 @@
         <v>298</v>
       </c>
       <c r="J66" s="31">
-        <f>6335*10000000</f>
-        <v>63350000000</v>
+        <f>6335*10^6</f>
+        <v>6335000000</v>
       </c>
       <c r="K66" s="31"/>
       <c r="L66" s="19" t="s">
@@ -4263,8 +4263,8 @@
         <v>1273</v>
       </c>
       <c r="J67" s="31">
-        <f>774*10000000</f>
-        <v>7740000000</v>
+        <f>774*10^6</f>
+        <v>774000000</v>
       </c>
       <c r="K67" s="31"/>
       <c r="L67" s="19" t="s">
@@ -4304,8 +4304,8 @@
         <v>298</v>
       </c>
       <c r="J68" s="31">
-        <f>6031*10000000</f>
-        <v>60310000000</v>
+        <f>6031*10^6</f>
+        <v>6031000000</v>
       </c>
       <c r="K68" s="31"/>
       <c r="L68" s="19" t="s">
@@ -4348,8 +4348,8 @@
         <v>1273</v>
       </c>
       <c r="J69" s="31">
-        <f>762*10000000</f>
-        <v>7620000000</v>
+        <f>762*10^6</f>
+        <v>762000000</v>
       </c>
       <c r="K69" s="31"/>
       <c r="L69" s="19" t="s">
@@ -5990,6 +5990,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -6004,11 +6009,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Small fix to `24-10_Contributions`
</commit_message>
<xml_diff>
--- a/24-10_Contributions.xlsx
+++ b/24-10_Contributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardonpa/Library/CloudStorage/GoogleDrive-ricardo.npa@gmail.com/Shared drives/Development/Codes/ULTERA-contribute-rdamaral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0119AE11-2942-EC4B-8509-6BC50BE494A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5E67E2-A570-C24A-AFFC-A007C03DB508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="107">
   <si>
     <t>Name:</t>
   </si>
@@ -414,9 +414,6 @@
   </si>
   <si>
     <t>10.1016/j.intermet.2024.108515</t>
-  </si>
-  <si>
-    <t>&gt;30</t>
   </si>
   <si>
     <t>T4</t>
@@ -1123,6 +1120,33 @@
     <xf numFmtId="11" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1174,34 +1198,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1487,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView tabSelected="1" topLeftCell="C42" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1523,19 +1520,19 @@
       <c r="B2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="41"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="50"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1545,17 +1542,17 @@
       <c r="B3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="43"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1573,43 +1570,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="57" t="s">
+      <c r="D5" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="57" t="s">
+      <c r="F5" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="57" t="s">
+      <c r="L5" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="57" t="s">
+      <c r="N5" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="40" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1620,19 +1617,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="57"/>
-      <c r="E6" s="57"/>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="57"/>
-      <c r="O6" s="60"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1677,7 +1674,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="61"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -1690,35 +1687,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="48" t="s">
+      <c r="B8" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="51" t="s">
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="52"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="52"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="54" t="s">
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="55"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="62" t="s">
+      <c r="P8" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="64"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="45"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1871,7 +1868,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>68</v>
@@ -1915,7 +1912,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>68</v>
@@ -1957,7 +1954,7 @@
         <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>68</v>
@@ -2001,7 +1998,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>68</v>
@@ -2127,7 +2124,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>68</v>
@@ -2169,7 +2166,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>68</v>
@@ -2211,7 +2208,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>68</v>
@@ -2253,7 +2250,7 @@
         <v>82</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>68</v>
@@ -2643,7 +2640,7 @@
         <v>87</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>72</v>
@@ -2687,7 +2684,7 @@
         <v>87</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>72</v>
@@ -2731,7 +2728,7 @@
         <v>87</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>72</v>
@@ -2774,7 +2771,7 @@
         <v>87</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>72</v>
@@ -2817,7 +2814,7 @@
         <v>87</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C34" s="33" t="s">
         <v>72</v>
@@ -2861,7 +2858,7 @@
         <v>87</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>72</v>
@@ -2905,7 +2902,7 @@
         <v>87</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>72</v>
@@ -2948,7 +2945,7 @@
         <v>87</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>72</v>
@@ -2991,7 +2988,7 @@
         <v>87</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>72</v>
@@ -3035,7 +3032,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>72</v>
@@ -3079,7 +3076,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>72</v>
@@ -3122,7 +3119,7 @@
         <v>87</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>72</v>
@@ -3165,7 +3162,7 @@
         <v>87</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>72</v>
@@ -3209,7 +3206,7 @@
         <v>87</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>72</v>
@@ -3253,7 +3250,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>72</v>
@@ -3296,7 +3293,7 @@
         <v>87</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>72</v>
@@ -3339,7 +3336,7 @@
         <v>87</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>72</v>
@@ -3383,7 +3380,7 @@
         <v>87</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>72</v>
@@ -3427,7 +3424,7 @@
         <v>87</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>72</v>
@@ -3470,7 +3467,7 @@
         <v>87</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>72</v>
@@ -3513,7 +3510,7 @@
         <v>87</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>72</v>
@@ -3557,7 +3554,7 @@
         <v>87</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>72</v>
@@ -3601,7 +3598,7 @@
         <v>87</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>72</v>
@@ -3644,7 +3641,7 @@
         <v>87</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>72</v>
@@ -3842,8 +3839,8 @@
         <f>1200+273</f>
         <v>1473</v>
       </c>
-      <c r="J57" s="31" t="s">
-        <v>96</v>
+      <c r="J57" s="31">
+        <v>30</v>
       </c>
       <c r="K57" s="31"/>
       <c r="L57" s="19" t="s">
@@ -3928,8 +3925,8 @@
         <f>1600+273</f>
         <v>1873</v>
       </c>
-      <c r="J59" s="31" t="s">
-        <v>96</v>
+      <c r="J59" s="31">
+        <v>30</v>
       </c>
       <c r="K59" s="31"/>
       <c r="L59" s="19" t="s">
@@ -4014,8 +4011,8 @@
         <f>1800+273</f>
         <v>2073</v>
       </c>
-      <c r="J61" s="31" t="s">
-        <v>96</v>
+      <c r="J61" s="31">
+        <v>30</v>
       </c>
       <c r="K61" s="31"/>
       <c r="L61" s="19" t="s">
@@ -4062,7 +4059,7 @@
         <v>44</v>
       </c>
       <c r="M62" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N62" s="19" t="s">
         <v>95</v>
@@ -4101,7 +4098,7 @@
         <v>81</v>
       </c>
       <c r="M63" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N63" s="19" t="s">
         <v>95</v>
@@ -4198,10 +4195,10 @@
         <v>4</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D66" s="32" t="s">
         <v>75</v>
@@ -4230,7 +4227,7 @@
         <v>84</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4238,10 +4235,10 @@
         <v>4</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D67" s="32" t="s">
         <v>75</v>
@@ -4271,10 +4268,10 @@
         <v>44</v>
       </c>
       <c r="M67" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="N67" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="N67" s="19" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4282,10 +4279,10 @@
         <v>4</v>
       </c>
       <c r="B68" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="33" t="s">
         <v>98</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>99</v>
       </c>
       <c r="D68" s="32" t="s">
         <v>75</v>
@@ -4315,7 +4312,7 @@
         <v>84</v>
       </c>
       <c r="N68" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4323,10 +4320,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C69" s="33" t="s">
         <v>98</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>99</v>
       </c>
       <c r="D69" s="32" t="s">
         <v>75</v>
@@ -4356,10 +4353,10 @@
         <v>44</v>
       </c>
       <c r="M69" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="N69" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="N69" s="19" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -5990,11 +5987,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -6009,6 +6001,11 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Change "total compressive ductility" to "compressive ductility"
</commit_message>
<xml_diff>
--- a/24-10_Contributions.xlsx
+++ b/24-10_Contributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricardonpa/Library/CloudStorage/GoogleDrive-ricardo.npa@gmail.com/Shared drives/Development/Codes/ULTERA-contribute-rdamaral/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5E67E2-A570-C24A-AFFC-A007C03DB508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A515584E-37FE-4E4C-9A09-C8572C591D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="106">
   <si>
     <t>Name:</t>
   </si>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>Nb Mo Ta W</t>
-  </si>
-  <si>
-    <t>total compressive ductility</t>
   </si>
   <si>
     <t>10.1016/j.intermet.2024.108515</t>
@@ -1120,6 +1117,63 @@
     <xf numFmtId="11" fontId="4" fillId="4" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1138,67 +1192,10 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1484,8 +1481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J62" sqref="J62"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1520,19 +1517,19 @@
       <c r="B2" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="54"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="50"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="41"/>
       <c r="O2" s="24"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1542,17 +1539,17 @@
       <c r="B3" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
-      <c r="K3" s="51"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="52"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
       <c r="O3" s="24"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1570,43 +1567,43 @@
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="C5" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="46" t="s">
+      <c r="F5" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="46" t="s">
+      <c r="I5" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="66" t="s">
+      <c r="J5" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="46" t="s">
+      <c r="L5" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="46" t="s">
+      <c r="M5" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="40" t="s">
+      <c r="O5" s="59" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1617,19 +1614,19 @@
       <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="48"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="66"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="46"/>
-      <c r="O6" s="41"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="57"/>
+      <c r="O6" s="60"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1674,7 +1671,7 @@
       <c r="N7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="61"/>
       <c r="P7" s="30" t="s">
         <v>40</v>
       </c>
@@ -1687,35 +1684,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="63" t="s">
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="N8" s="64"/>
+      <c r="N8" s="55"/>
       <c r="O8" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="43" t="s">
+      <c r="P8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="45"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="64"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -1868,7 +1865,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>68</v>
@@ -1912,7 +1909,7 @@
         <v>82</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>68</v>
@@ -1954,7 +1951,7 @@
         <v>82</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="32" t="s">
         <v>68</v>
@@ -1998,7 +1995,7 @@
         <v>82</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C15" s="32" t="s">
         <v>68</v>
@@ -2124,7 +2121,7 @@
         <v>82</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>68</v>
@@ -2166,7 +2163,7 @@
         <v>82</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="32" t="s">
         <v>68</v>
@@ -2208,7 +2205,7 @@
         <v>82</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>68</v>
@@ -2250,7 +2247,7 @@
         <v>82</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>68</v>
@@ -2640,7 +2637,7 @@
         <v>87</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>72</v>
@@ -2684,7 +2681,7 @@
         <v>87</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="33" t="s">
         <v>72</v>
@@ -2728,7 +2725,7 @@
         <v>87</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="33" t="s">
         <v>72</v>
@@ -2771,7 +2768,7 @@
         <v>87</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" s="33" t="s">
         <v>72</v>
@@ -2814,7 +2811,7 @@
         <v>87</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" s="33" t="s">
         <v>72</v>
@@ -2858,7 +2855,7 @@
         <v>87</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" s="33" t="s">
         <v>72</v>
@@ -2902,7 +2899,7 @@
         <v>87</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" s="33" t="s">
         <v>72</v>
@@ -2945,7 +2942,7 @@
         <v>87</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C37" s="33" t="s">
         <v>72</v>
@@ -2988,7 +2985,7 @@
         <v>87</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C38" s="33" t="s">
         <v>72</v>
@@ -3032,7 +3029,7 @@
         <v>87</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C39" s="33" t="s">
         <v>72</v>
@@ -3076,7 +3073,7 @@
         <v>87</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C40" s="33" t="s">
         <v>72</v>
@@ -3119,7 +3116,7 @@
         <v>87</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="33" t="s">
         <v>72</v>
@@ -3162,7 +3159,7 @@
         <v>87</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C42" s="33" t="s">
         <v>72</v>
@@ -3206,7 +3203,7 @@
         <v>87</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C43" s="33" t="s">
         <v>72</v>
@@ -3250,7 +3247,7 @@
         <v>87</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="33" t="s">
         <v>72</v>
@@ -3293,7 +3290,7 @@
         <v>87</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C45" s="33" t="s">
         <v>72</v>
@@ -3336,7 +3333,7 @@
         <v>87</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>72</v>
@@ -3380,7 +3377,7 @@
         <v>87</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C47" s="33" t="s">
         <v>72</v>
@@ -3424,7 +3421,7 @@
         <v>87</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C48" s="33" t="s">
         <v>72</v>
@@ -3467,7 +3464,7 @@
         <v>87</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C49" s="33" t="s">
         <v>72</v>
@@ -3510,7 +3507,7 @@
         <v>87</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C50" s="33" t="s">
         <v>72</v>
@@ -3554,7 +3551,7 @@
         <v>87</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>72</v>
@@ -3598,7 +3595,7 @@
         <v>87</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>72</v>
@@ -3641,7 +3638,7 @@
         <v>87</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>72</v>
@@ -3721,7 +3718,7 @@
         <v>79</v>
       </c>
       <c r="N54" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -3739,7 +3736,7 @@
       </c>
       <c r="E55" s="19"/>
       <c r="F55" s="32" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G55" s="32" t="s">
         <v>19</v>
@@ -3764,7 +3761,7 @@
         <v>79</v>
       </c>
       <c r="N55" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -3809,7 +3806,7 @@
         <v>79</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3827,7 +3824,7 @@
       </c>
       <c r="E57" s="19"/>
       <c r="F57" s="32" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G57" s="32" t="s">
         <v>19</v>
@@ -3850,7 +3847,7 @@
         <v>79</v>
       </c>
       <c r="N57" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -3895,7 +3892,7 @@
         <v>79</v>
       </c>
       <c r="N58" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -3913,7 +3910,7 @@
       </c>
       <c r="E59" s="19"/>
       <c r="F59" s="32" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G59" s="32" t="s">
         <v>19</v>
@@ -3936,7 +3933,7 @@
         <v>79</v>
       </c>
       <c r="N59" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -3981,7 +3978,7 @@
         <v>79</v>
       </c>
       <c r="N60" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
@@ -3999,7 +3996,7 @@
       </c>
       <c r="E61" s="19"/>
       <c r="F61" s="32" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G61" s="32" t="s">
         <v>19</v>
@@ -4022,7 +4019,7 @@
         <v>79</v>
       </c>
       <c r="N61" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -4059,10 +4056,10 @@
         <v>44</v>
       </c>
       <c r="M62" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N62" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
@@ -4098,10 +4095,10 @@
         <v>81</v>
       </c>
       <c r="M63" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N63" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
@@ -4145,7 +4142,7 @@
         <v>79</v>
       </c>
       <c r="N64" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -4162,7 +4159,7 @@
         <v>61</v>
       </c>
       <c r="F65" s="32" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="G65" s="32" t="s">
         <v>19</v>
@@ -4187,7 +4184,7 @@
         <v>79</v>
       </c>
       <c r="N65" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -4195,10 +4192,10 @@
         <v>4</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C66" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D66" s="32" t="s">
         <v>75</v>
@@ -4227,7 +4224,7 @@
         <v>84</v>
       </c>
       <c r="N66" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4235,10 +4232,10 @@
         <v>4</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C67" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D67" s="32" t="s">
         <v>75</v>
@@ -4268,10 +4265,10 @@
         <v>44</v>
       </c>
       <c r="M67" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="N67" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="N67" s="19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4279,10 +4276,10 @@
         <v>4</v>
       </c>
       <c r="B68" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="33" t="s">
         <v>97</v>
-      </c>
-      <c r="C68" s="33" t="s">
-        <v>98</v>
       </c>
       <c r="D68" s="32" t="s">
         <v>75</v>
@@ -4312,7 +4309,7 @@
         <v>84</v>
       </c>
       <c r="N68" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4320,10 +4317,10 @@
         <v>4</v>
       </c>
       <c r="B69" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="C69" s="33" t="s">
         <v>97</v>
-      </c>
-      <c r="C69" s="33" t="s">
-        <v>98</v>
       </c>
       <c r="D69" s="32" t="s">
         <v>75</v>
@@ -4353,10 +4350,10 @@
         <v>44</v>
       </c>
       <c r="M69" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="N69" s="19" t="s">
         <v>99</v>
-      </c>
-      <c r="N69" s="19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -5987,6 +5984,11 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -6001,11 +6003,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>

</xml_diff>